<commit_message>
Últimas mudanças no PCCTI
</commit_message>
<xml_diff>
--- a/Docs/Controle CTI_QRD.xlsx
+++ b/Docs/Controle CTI_QRD.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Cronograma BI QRD" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plano de ação'!$A$6:$L$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plano de ação'!$A$6:$M$26</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="147">
   <si>
     <t>Item</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>BI</t>
-  </si>
-  <si>
-    <t>Análise de Valores carregados no BI</t>
-  </si>
-  <si>
-    <t>Processo formal de conferência de dados carregados, com fluxo definido e evidência catalogadas</t>
   </si>
   <si>
     <t>Precisa ser apresentado durante sprint 25</t>
@@ -396,9 +390,6 @@
     <t>Denis/André Duarte</t>
   </si>
   <si>
-    <t>24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
-  </si>
-  <si>
     <t>Em avaliação</t>
   </si>
   <si>
@@ -431,6 +422,76 @@
 27/07/18 - Modelo de dados entregue pela equipe de BI e sob avaliação da equipe PSV.
 24/07/18 - O modelo foi solicitado novamente em reunião com equipe de BI e TI QRD, fundamental para conclusão do módulo de SLA
 03/07/18 - Foi definido em reunião com equipes de TI que a base de dados origem para Interface pública será a Stage 1, e portanto foi solicitado novamente o Diagrama para avaliação da TI PSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trecho de mail enviado em 05/07 p/ esclarecimento da entrega
+---------------------------------------------------------------------
+Interface pública
+1) Foi solicitada a criação da interface púbica de acesso aos dados do Planserv. 
+2) Ficou acordado a criação de um ambiente com uma "cópia simplificada" do banco de dados do Planserv, com latência de 1 dia, contendo apenas as informações relacionadas aos requisitos de negócio. Tal ambiente seria acessível através de VPN, separadamente do ambiente operacional do Plano. 
+3) A Qualirede irá enviar à TI da Planserv documentação sobre as principais entidades que deverão compor está base de dados. O Planserv irá avaliar o modelo para, eventualmente, sugerir alterações. Após aprovação do Planserv, será iniciado o processo de construção/ajustes das rotinas de copia dos dados. 
+</t>
+  </si>
+  <si>
+    <t>PLN 91</t>
+  </si>
+  <si>
+    <t>Chamado</t>
+  </si>
+  <si>
+    <t>Relatório Glosa de Edital Março a Junho de 2018</t>
+  </si>
+  <si>
+    <t>Relatório para CG, sem atendimento desde criação em 18/07/18</t>
+  </si>
+  <si>
+    <t>Dados críticos para tomada de decisão da Coordenadora Geral</t>
+  </si>
+  <si>
+    <t>Dados de biometria</t>
+  </si>
+  <si>
+    <t>Realizar acompanhamento mensal</t>
+  </si>
+  <si>
+    <t>Controle de acesso de beneficiários, alta incidência de chamados em Call Center</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Extrato de Utilização</t>
+  </si>
+  <si>
+    <t>Informações sobre consumo, autoregulação pelos beneficiários</t>
+  </si>
+  <si>
+    <t>André Duarte</t>
+  </si>
+  <si>
+    <t>Análise de Valores carregados no BI (Auditoria do BI)</t>
+  </si>
+  <si>
+    <t>Ponto de controle crítico PSV</t>
+  </si>
+  <si>
+    <t>Processo formal de conferência de dados carregados, com fluxo definido e evidência catalogadas (Ponto de controle crítico PSV)</t>
+  </si>
+  <si>
+    <t>Gera Chamado?</t>
+  </si>
+  <si>
+    <t>31/07/18 - 
+24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
+  </si>
+  <si>
+    <t>PLN 84</t>
+  </si>
+  <si>
+    <t>Extração das informações Contas Abril e Maio /2018</t>
+  </si>
+  <si>
+    <t>Qualidade de atendimento do chamado</t>
   </si>
 </sst>
 </file>
@@ -874,32 +935,32 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,13 +1008,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>786493</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>53067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>2292473</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>224517</xdr:rowOff>
@@ -1273,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1284,18 +1345,19 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="10" width="18.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="56.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="27" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="56.42578125" customWidth="1"/>
+    <col min="13" max="13" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="45"/>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1">
+      <c r="A2" s="43"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1305,15 +1367,16 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="20"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="20"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="12" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="46"/>
+    <row r="3" spans="1:13" ht="22.5" customHeight="1">
+      <c r="A3" s="44"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1323,32 +1386,34 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="21"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="21"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="21"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A4" s="47"/>
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A4" s="45"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="8">
-        <v>43308</v>
+        <v>43311</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="22"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="22"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
+      <c r="K4" s="22"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="31.5">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1368,25 +1433,28 @@
         <v>3</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="J6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>29</v>
+      <c r="K6" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="L6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="195">
+    <row r="7" spans="1:13" ht="240">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -1399,30 +1467,33 @@
       <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="44" t="s">
-        <v>122</v>
+      <c r="E7" s="42" t="s">
+        <v>119</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="26">
+      <c r="K7" s="26">
         <v>43312</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" spans="1:12" ht="180">
+      <c r="L7" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="165">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1442,142 +1513,146 @@
         <v>13</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="26">
+      <c r="K8" s="26">
         <v>43312</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="120">
+      <c r="L8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="90">
       <c r="A9" s="7">
         <v>3</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="26">
+      <c r="J9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="26">
         <v>43312</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="75">
+      <c r="L9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" ht="75">
       <c r="A10" s="7">
         <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="26">
-        <v>43312</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="225">
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" ht="210">
       <c r="A11" s="7">
         <v>5</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="26">
+      <c r="J11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="26">
         <v>43312</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="240">
+      <c r="L11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" ht="210">
       <c r="A12" s="7">
         <v>6</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>19</v>
@@ -1586,303 +1661,394 @@
         <v>13</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="26">
+        <v>55</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="26">
         <v>43312</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="45">
+      <c r="L12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" ht="45">
       <c r="A13" s="7">
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="26">
-        <v>43312</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="75">
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" ht="60">
       <c r="A14" s="7">
         <v>8</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="40" t="s">
+      <c r="L14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="75">
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" ht="75">
       <c r="A15" s="7">
         <v>9</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" spans="1:12" ht="90">
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" ht="90">
       <c r="A16" s="7">
         <v>10</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="26">
+      <c r="K16" s="26">
         <v>43312</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:12" ht="105">
+      <c r="L16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" ht="105">
       <c r="A17" s="7">
         <v>11</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="J17" s="26">
+      <c r="J17" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="26">
         <v>43312</v>
       </c>
-      <c r="K17" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" spans="1:12" ht="45">
+      <c r="L17" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" ht="45">
       <c r="A18" s="7">
         <v>12</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="J18" s="26">
+      <c r="K18" s="26">
         <v>43312</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" spans="1:12" ht="30.75" customHeight="1">
+      <c r="L18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" ht="60">
       <c r="A19" s="7">
         <v>13</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-    </row>
-    <row r="20" spans="1:12" ht="30.75" customHeight="1">
+      <c r="B19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" ht="60">
       <c r="A20" s="7">
         <v>14</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" spans="1:12" ht="30.75" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" ht="75">
       <c r="A21" s="7">
         <v>15</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-    </row>
-    <row r="22" spans="1:12" ht="30.75" customHeight="1">
+      <c r="B21" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="K21" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" ht="60">
       <c r="A22" s="7">
         <v>16</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-    </row>
-    <row r="23" spans="1:12" ht="30.75" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="26">
+        <v>43312</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" ht="30.75" customHeight="1">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -1892,13 +2058,14 @@
       <c r="E23" s="16"/>
       <c r="F23" s="7"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="11"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="24"/>
       <c r="L23" s="11"/>
-    </row>
-    <row r="24" spans="1:12" ht="30.75" customHeight="1">
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" ht="30.75" customHeight="1">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -1908,13 +2075,14 @@
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="11"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="24"/>
       <c r="L24" s="11"/>
-    </row>
-    <row r="25" spans="1:12" ht="30.75" customHeight="1">
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" ht="30.75" customHeight="1">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1924,13 +2092,14 @@
       <c r="E25" s="16"/>
       <c r="F25" s="7"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="11"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="24"/>
       <c r="L25" s="11"/>
-    </row>
-    <row r="26" spans="1:12" ht="30.75" customHeight="1">
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" ht="30.75" customHeight="1">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1940,17 +2109,20 @@
       <c r="E26" s="16"/>
       <c r="F26" s="7"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="11"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:L26"/>
+  <autoFilter ref="A6:M26">
+    <filterColumn colId="7"/>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -1980,43 +2152,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75">
-      <c r="A1" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="A1" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="31.5">
       <c r="A2" s="32"/>
       <c r="B2" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="E2" s="33" t="s">
         <v>62</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>65</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2024,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="36">
         <v>43283</v>
@@ -2036,10 +2208,10 @@
         <v>43284</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="35"/>
@@ -2049,10 +2221,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="36">
         <v>43283</v>
@@ -2061,10 +2233,10 @@
         <v>43284</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="35"/>
@@ -2074,10 +2246,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="36">
         <v>43285</v>
@@ -2087,10 +2259,10 @@
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I5" s="35"/>
     </row>
@@ -2099,10 +2271,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="36">
         <v>43286</v>
@@ -2112,7 +2284,7 @@
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="35"/>
@@ -2122,10 +2294,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="36">
         <v>43284</v>
@@ -2135,10 +2307,10 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7" s="35"/>
     </row>
@@ -2147,10 +2319,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="36">
         <v>43287</v>
@@ -2159,10 +2331,10 @@
         <v>43287</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="35"/>
@@ -2172,10 +2344,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="36">
         <v>43305</v>
@@ -2186,7 +2358,7 @@
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I9" s="35"/>
     </row>
@@ -2195,10 +2367,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="36">
         <v>43305</v>
@@ -2208,10 +2380,10 @@
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I10" s="35"/>
     </row>
@@ -2220,10 +2392,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="36">
         <v>43271</v>
@@ -2232,10 +2404,10 @@
         <v>43271</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="35"/>
@@ -2245,10 +2417,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="36">
         <v>43271</v>
@@ -2257,10 +2429,10 @@
         <v>43271</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H12" s="30"/>
       <c r="I12" s="35"/>
@@ -2270,10 +2442,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D13" s="36">
         <v>43278</v>
@@ -2282,13 +2454,13 @@
         <v>43315</v>
       </c>
       <c r="F13" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="30" t="s">
         <v>90</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>92</v>
       </c>
       <c r="I13" s="35"/>
     </row>
@@ -2297,10 +2469,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="36">
         <v>43290</v>
@@ -2309,10 +2481,10 @@
         <v>43294</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="35"/>
@@ -2322,10 +2494,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" s="36">
         <v>43297</v>
@@ -2334,13 +2506,13 @@
         <v>43315</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I15" s="35"/>
     </row>
@@ -2349,10 +2521,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D16" s="36">
         <v>43318</v>
@@ -2370,10 +2542,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" s="36">
         <v>43280</v>
@@ -2382,13 +2554,13 @@
         <v>43313</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I17" s="35"/>
     </row>

</xml_diff>